<commit_message>
Improve mission expense calculation and data handling
Refactor mission expense calculation logic, update TypeScript types for Mission and ExpenseItem, and adjust the BankDistribution component props. Also includes an update to the tsx dependency in package.json and minor corrections in excel-storage.ts for handling expenses and bank data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/28fb3125-3207-48c3-a350-c46c2aff26ea/7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407/gf3PQPA
</commit_message>
<xml_diff>
--- a/data/missions.xlsx
+++ b/data/missions.xlsx
@@ -448,7 +448,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>766b62c0-67c4-48b4-9afb-5340047dabab</v>
+        <v>61c7f0c7-0e18-48c0-920b-80de376e6d9c</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="str">
-        <v>2025-09-14T10:04:43.016Z</v>
+        <v>2025-09-14T10:18:58.085Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimize mission management by preventing unnecessary updates
This commit refactors the mission management component by wrapping several handler functions (updateActiveMission, handleEmployeeChange, handleMissionDateChange, handleStatementChange, addExpenseItem, updateExpenseItem, removeExpenseItem) in useCallback to optimize performance and prevent redundant data mutations and API calls. It also includes an equality guard in updateActiveMission to ensure updates only occur when there are actual changes, further optimizing the process. The useEffect dependency array in the employee-lookup component was also adjusted to prevent potential infinite loops.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/28fb3125-3207-48c3-a350-c46c2aff26ea/7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407/ocF4Dnk
</commit_message>
<xml_diff>
--- a/data/missions.xlsx
+++ b/data/missions.xlsx
@@ -451,13 +451,13 @@
         <v>61c7f0c7-0e18-48c0-920b-80de376e6d9c</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>محمد مجدى السيد عبد الدايم</v>
       </c>
       <c r="D2" t="str">
-        <v/>
+        <v>20أ القاهرة</v>
       </c>
       <c r="E2" t="str">
         <v>2025-09-14</v>

</xml_diff>

<commit_message>
Remove save confirmation popups and fix button nesting issues
Removes the "Changes saved" toast notification on successful mission updates and resolves a `validateDOMNesting` error related to nested buttons in the mission management component. Also updates the styling and structure of mission tabs and delete buttons.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/28fb3125-3207-48c3-a350-c46c2aff26ea/7c6c047e-2b2a-48cc-8b30-5ecb0e6eb407/ocF4Dnk
</commit_message>
<xml_diff>
--- a/data/missions.xlsx
+++ b/data/missions.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -451,10 +451,10 @@
         <v>61c7f0c7-0e18-48c0-920b-80de376e6d9c</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C2" t="str">
-        <v>محمد مجدى السيد عبد الدايم</v>
+        <v>عبد العزيز صلاح عبد العزيز على حسن</v>
       </c>
       <c r="D2" t="str">
         <v>20أ القاهرة</v>
@@ -463,18 +463,70 @@
         <v>2025-09-14</v>
       </c>
       <c r="H2" t="str">
-        <v>[]</v>
+        <v>[{"id":"expense-1","type":"transportation","amount":100,"banks":["كريدى","مانى فيللوز"]},{"id":"expense-2","type":"transportation","amount":30,"banks":["اسكندرية"]},{"id":"expense-3","type":"hospitality","amount":0,"banks":[]},{"id":"expense-4","type":"fees","amount":0,"banks":[]}]</v>
       </c>
       <c r="I2" t="str">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="J2" t="str">
         <v>2025-09-14T10:18:58.085Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0e3f0a1e-d8a6-44df-b229-03628e5bca16</v>
+      </c>
+      <c r="B3">
+        <v>62</v>
+      </c>
+      <c r="C3" t="str">
+        <v>محمد مجدى السيد عبد الدايم</v>
+      </c>
+      <c r="D3" t="str">
+        <v>20أ القاهرة</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2025-09-14</v>
+      </c>
+      <c r="H3" t="str">
+        <v>[{"id":"expense-1","type":"fees","amount":50,"banks":["كريدى","مانى فيللوز"]},{"id":"expense-2","type":"fees","amount":50,"banks":["كريدى"]}]</v>
+      </c>
+      <c r="I3" t="str">
+        <v>100</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2025-09-14T11:31:03.321Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6c41556f-a921-4153-bbf5-ec5a27eb2838</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-09-14</v>
+      </c>
+      <c r="H4" t="str">
+        <v>[]</v>
+      </c>
+      <c r="I4" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2025-09-14T11:31:55.900Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improve mission statement input to reduce typing lag
Introduce debounced updates for mission statement and other fields to prevent UI lag during user input.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0ef20dd9-bf40-4a82-beea-3f8c2245df5c
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4b3b2a39-3d0e-4428-9c27-7e63726dfdd6/0ef20dd9-bf40-4a82-beea-3f8c2245df5c/qnef9ZW
</commit_message>
<xml_diff>
--- a/data/missions.xlsx
+++ b/data/missions.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,10 +463,10 @@
         <v>2025-09-14</v>
       </c>
       <c r="H2" t="str">
-        <v>[{"id":"expense-1","type":"transportation","amount":100,"banks":["كريدى","مانى فيللوز"]},{"id":"expense-2","type":"transportation","amount":300,"banks":["اسكندرية"]}]</v>
+        <v>[{"id":"expense-1","type":"transportation","amount":0.01,"banks":["كريدى","مانى فيللوز"]},{"id":"expense-2","type":"transportation","amount":300,"banks":["اسكندرية"]}]</v>
       </c>
       <c r="I2" t="str">
-        <v>400</v>
+        <v>300.01</v>
       </c>
       <c r="J2" t="str">
         <v>2025-09-14T10:18:58.085Z</v>
@@ -498,9 +498,38 @@
         <v>2025-09-14T11:31:03.321Z</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>3f65f14e-3669-4aa4-8858-3a66a39cef52</v>
+      </c>
+      <c r="B4">
+        <v>675</v>
+      </c>
+      <c r="C4" t="str">
+        <v>كريم خالد محمد محمود</v>
+      </c>
+      <c r="D4" t="str">
+        <v>20أ القاهرة</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-09-26</v>
+      </c>
+      <c r="G4" t="str">
+        <v>تتيستسس</v>
+      </c>
+      <c r="H4" t="str">
+        <v>[{"id":"expense-1","type":"transportation","amount":10,"banks":["كريدى","مانى فيللوز"]}]</v>
+      </c>
+      <c r="I4" t="str">
+        <v>10</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2025-09-14T12:02:06.872Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improve application responsiveness by adjusting input delays
Adjusted debounce delay for mission updates to 2000ms and disabled automatic Excel saving to enhance performance.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0ef20dd9-bf40-4a82-beea-3f8c2245df5c
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4b3b2a39-3d0e-4428-9c27-7e63726dfdd6/0ef20dd9-bf40-4a82-beea-3f8c2245df5c/Nm5Rb6b
</commit_message>
<xml_diff>
--- a/data/missions.xlsx
+++ b/data/missions.xlsx
@@ -463,10 +463,10 @@
         <v>2025-09-14</v>
       </c>
       <c r="H2" t="str">
-        <v>[{"id":"expense-1","type":"transportation","amount":0.01,"banks":["كريدى","مانى فيللوز"]},{"id":"expense-2","type":"transportation","amount":300,"banks":["اسكندرية"]}]</v>
+        <v>[{"id":"expense-2","type":"transportation","amount":300,"banks":["اسكندرية"]},{"id":"expense-3","type":"office-supplies","amount":55,"banks":[]}]</v>
       </c>
       <c r="I2" t="str">
-        <v>300.01</v>
+        <v>355</v>
       </c>
       <c r="J2" t="str">
         <v>2025-09-14T10:18:58.085Z</v>

</xml_diff>